<commit_message>
v6.6 zmiana wagi i wzrostu
*Dodano możliwość zmiany wagi

*Dodano możliwość zmiany wzrostu

* dodatkowy excel i poprawki
</commit_message>
<xml_diff>
--- a/excel/wzrostomierz.xlsx
+++ b/excel/wzrostomierz.xlsx
@@ -19,15 +19,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>data</t>
   </si>
   <si>
     <t>id_klienta</t>
-  </si>
-  <si>
-    <t>0</t>
   </si>
   <si>
     <t>2020-12-16</t>
@@ -43,6 +40,24 @@
   </si>
   <si>
     <t>150</t>
+  </si>
+  <si>
+    <t>waga</t>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>stopien_dolrzalosci</t>
+  </si>
+  <si>
+    <t>PHV</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>0.2</t>
   </si>
 </sst>
 </file>
@@ -353,7 +368,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -364,7 +379,7 @@
   <dimension ref="A1:J453"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D20"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -372,6 +387,7 @@
     <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -382,28 +398,43 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
+      <c r="F2" s="1" t="s">
+        <v>12</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>7</v>
+      <c r="G2" s="1" t="s">
+        <v>11</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="1"/>

</xml_diff>